<commit_message>
Update Halloween Game Jam 2025 (1).xlsx
</commit_message>
<xml_diff>
--- a/Assets/Levels/Halloween Game Jam 2025 (1).xlsx
+++ b/Assets/Levels/Halloween Game Jam 2025 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\BLO.OD.-PAC.T\Assets\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8084A-2E03-40AC-B979-1A9A950B69CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CFD312-B96F-4C98-97CE-4B3EF57CE225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2136" windowWidth="17280" windowHeight="8964" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task1.1" sheetId="21" r:id="rId1"/>

</xml_diff>